<commit_message>
Integration Dialogue Ernest et Léontine Act1D2
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION.xlsx
+++ b/Assets/StreamingAssets/TABLE_REFERENCE_LOCALISATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Act1Niv0" sheetId="1" r:id="rId1"/>
@@ -19894,7 +19894,7 @@
   </sheetPr>
   <dimension ref="A1:H311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+    <sheetView topLeftCell="A290" workbookViewId="0">
       <selection activeCell="F313" sqref="F313"/>
     </sheetView>
   </sheetViews>
@@ -27990,13 +27990,14 @@
   </sheetPr>
   <dimension ref="A1:H574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F572" sqref="F572"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>

</xml_diff>